<commit_message>
Plugins allow you to run a file through a compiler before mundle parses it For example, to include coffeescript or jade files. With tests, updated docs, and npm version bump.
</commit_message>
<xml_diff>
--- a/tests/benchmark/results/results.xlsx
+++ b/tests/benchmark/results/results.xlsx
@@ -4,10 +4,11 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22221"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="0" windowWidth="32960" windowHeight="24860" tabRatio="500"/>
+    <workbookView xWindow="420" yWindow="0" windowWidth="48720" windowHeight="28260" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -19,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="12">
   <si>
     <t>Concurrency</t>
   </si>
@@ -52,6 +53,9 @@
   </si>
   <si>
     <t>Mundle cache file contents 609a8bcce6a379ef5ba3a881e8d414550d5006cb</t>
+  </si>
+  <si>
+    <t>Mundlejs</t>
   </si>
 </sst>
 </file>
@@ -100,8 +104,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
@@ -112,9 +118,11 @@
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="5">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -596,11 +604,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2131459736"/>
-        <c:axId val="-2131189032"/>
+        <c:axId val="2036308920"/>
+        <c:axId val="2036314488"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2131459736"/>
+        <c:axId val="2036308920"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -629,7 +637,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2131189032"/>
+        <c:crossAx val="2036314488"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -637,7 +645,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2131189032"/>
+        <c:axId val="2036314488"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -667,9 +675,2144 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2131459736"/>
+        <c:crossAx val="2036308920"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="118"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="18"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="47625">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="diamond"/>
+            <c:size val="2"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet2!$A$3:$A$56</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="54"/>
+                <c:pt idx="0">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>20.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>30.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>40.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>50.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>60.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>70.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>80.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>90.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>100.0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>110.0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>120.0</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>130.0</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>140.0</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>150.0</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>160.0</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>170.0</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>180.0</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>190.0</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>200.0</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>210.0</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>220.0</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>230.0</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>240.0</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>250.0</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>260.0</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>270.0</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>280.0</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>290.0</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>300.0</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>310.0</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>320.0</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>330.0</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>340.0</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>350.0</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>360.0</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>370.0</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>380.0</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>390.0</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>400.0</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>410.0</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>420.0</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>430.0</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>440.0</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>450.0</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>460.0</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>470.0</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>480.0</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>490.0</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>500.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet2!$B$3:$B$56</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="54"/>
+                <c:pt idx="0">
+                  <c:v>154.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>157.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>152.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>152.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>152.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>152.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>152.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>151.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>154.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>154.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>153.0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>151.0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>150.0</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>151.0</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>148.0</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>147.0</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>143.0</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>143.0</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>145.0</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>146.0</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>146.0</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>147.0</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>148.0</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>148.0</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>147.0</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>147.0</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>145.0</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>142.0</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>142.0</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>142.0</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>145.0</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>146.0</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>147.0</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>147.0</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>148.0</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>150.0</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>150.0</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>149.0</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>147.0</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>147.0</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>152.0</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>150.0</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>146.0</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>147.0</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>148.0</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>152.0</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>156.0</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>154.0</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>154.0</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>155.0</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>154.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:spPr>
+            <a:ln w="47625">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="6"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet2!$A$3:$A$56</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="54"/>
+                <c:pt idx="0">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>20.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>30.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>40.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>50.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>60.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>70.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>80.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>90.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>100.0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>110.0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>120.0</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>130.0</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>140.0</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>150.0</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>160.0</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>170.0</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>180.0</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>190.0</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>200.0</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>210.0</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>220.0</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>230.0</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>240.0</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>250.0</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>260.0</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>270.0</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>280.0</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>290.0</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>300.0</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>310.0</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>320.0</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>330.0</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>340.0</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>350.0</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>360.0</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>370.0</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>380.0</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>390.0</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>400.0</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>410.0</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>420.0</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>430.0</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>440.0</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>450.0</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>460.0</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>470.0</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>480.0</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>490.0</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>500.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet2!$C$3:$C$56</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="54"/>
+                <c:pt idx="0">
+                  <c:v>159.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>158.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>152.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>153.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>153.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>153.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>153.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>152.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>154.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>154.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>154.0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>152.0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>150.0</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>151.0</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>148.0</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>147.0</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>145.0</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>144.0</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>145.0</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>146.0</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>147.0</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>148.0</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>148.0</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>148.0</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>148.0</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>147.0</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>146.0</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>143.0</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>142.0</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>147.0</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>148.0</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>147.0</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>148.0</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>147.0</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>149.0</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>151.0</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>151.0</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>150.0</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>148.0</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>149.0</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>153.0</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>152.0</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>148.0</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>148.0</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>150.0</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>154.0</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>157.0</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>155.0</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>154.0</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>155.0</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>155.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:spPr>
+            <a:ln w="47625">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="square"/>
+            <c:size val="2"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet2!$A$3:$A$56</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="54"/>
+                <c:pt idx="0">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>20.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>30.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>40.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>50.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>60.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>70.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>80.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>90.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>100.0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>110.0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>120.0</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>130.0</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>140.0</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>150.0</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>160.0</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>170.0</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>180.0</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>190.0</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>200.0</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>210.0</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>220.0</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>230.0</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>240.0</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>250.0</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>260.0</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>270.0</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>280.0</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>290.0</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>300.0</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>310.0</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>320.0</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>330.0</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>340.0</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>350.0</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>360.0</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>370.0</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>380.0</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>390.0</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>400.0</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>410.0</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>420.0</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>430.0</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>440.0</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>450.0</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>460.0</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>470.0</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>480.0</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>490.0</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>500.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet2!$D$3:$D$56</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="54"/>
+                <c:pt idx="0">
+                  <c:v>163.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>160.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>154.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>154.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>154.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>155.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>156.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>154.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>155.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>155.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>155.0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>154.0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>151.0</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>152.0</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>150.0</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>148.0</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>146.0</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>145.0</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>146.0</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>148.0</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>149.0</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>149.0</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>149.0</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>150.0</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>150.0</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>148.0</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>147.0</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>144.0</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>143.0</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>150.0</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>151.0</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>150.0</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>150.0</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>149.0</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>151.0</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>153.0</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>153.0</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>151.0</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>150.0</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>155.0</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>155.0</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>153.0</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>150.0</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>149.0</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>153.0</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>156.0</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>158.0</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>156.0</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>156.0</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>156.0</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>157.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:spPr>
+            <a:ln w="47625">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="square"/>
+            <c:size val="2"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet2!$A$3:$A$56</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="54"/>
+                <c:pt idx="0">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>20.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>30.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>40.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>50.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>60.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>70.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>80.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>90.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>100.0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>110.0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>120.0</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>130.0</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>140.0</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>150.0</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>160.0</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>170.0</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>180.0</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>190.0</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>200.0</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>210.0</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>220.0</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>230.0</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>240.0</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>250.0</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>260.0</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>270.0</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>280.0</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>290.0</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>300.0</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>310.0</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>320.0</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>330.0</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>340.0</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>350.0</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>360.0</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>370.0</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>380.0</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>390.0</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>400.0</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>410.0</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>420.0</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>430.0</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>440.0</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>450.0</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>460.0</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>470.0</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>480.0</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>490.0</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>500.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet2!$E$3:$E$56</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="54"/>
+                <c:pt idx="0">
+                  <c:v>139.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>164.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>163.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>156.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>158.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>158.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>158.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>159.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>159.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>158.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>158.0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>159.0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>159.0</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>159.0</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>159.0</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>158.0</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>157.0</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>158.0</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>157.0</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>156.0</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>156.0</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>154.0</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>155.0</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>155.0</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>157.0</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>157.0</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>157.0</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>156.0</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>156.0</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>155.0</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>149.0</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>150.0</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>144.0</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>143.0</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>147.0</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>152.0</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>152.0</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>153.0</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>155.0</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>156.0</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>156.0</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>157.0</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>166.0</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>164.0</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>164.0</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>160.0</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>159.0</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>159.0</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>160.0</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>155.0</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>161.0</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>160.0</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>161.0</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>160.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:spPr>
+            <a:ln w="47625">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="6"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet2!$A$3:$A$56</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="54"/>
+                <c:pt idx="0">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>20.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>30.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>40.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>50.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>60.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>70.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>80.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>90.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>100.0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>110.0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>120.0</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>130.0</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>140.0</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>150.0</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>160.0</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>170.0</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>180.0</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>190.0</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>200.0</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>210.0</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>220.0</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>230.0</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>240.0</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>250.0</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>260.0</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>270.0</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>280.0</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>290.0</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>300.0</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>310.0</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>320.0</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>330.0</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>340.0</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>350.0</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>360.0</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>370.0</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>380.0</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>390.0</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>400.0</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>410.0</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>420.0</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>430.0</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>440.0</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>450.0</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>460.0</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>470.0</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>480.0</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>490.0</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>500.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet2!$F$3:$F$56</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="54"/>
+                <c:pt idx="0">
+                  <c:v>155.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>166.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>164.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>160.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>160.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>158.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>158.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>159.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>160.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>158.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>158.0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>159.0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>159.0</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>160.0</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>159.0</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>158.0</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>158.0</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>158.0</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>157.0</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>156.0</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>157.0</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>156.0</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>156.0</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>156.0</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>157.0</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>158.0</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>157.0</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>156.0</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>156.0</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>155.0</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>151.0</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>151.0</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>148.0</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>147.0</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>149.0</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>153.0</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>154.0</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>155.0</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>156.0</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>157.0</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>158.0</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>164.0</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>167.0</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>166.0</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>164.0</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>162.0</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>160.0</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>160.0</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>161.0</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>158.0</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>161.0</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>162.0</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>163.0</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>163.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="5"/>
+          <c:spPr>
+            <a:ln w="47625">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="square"/>
+            <c:size val="2"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet2!$A$3:$A$56</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="54"/>
+                <c:pt idx="0">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>20.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>30.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>40.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>50.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>60.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>70.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>80.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>90.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>100.0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>110.0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>120.0</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>130.0</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>140.0</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>150.0</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>160.0</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>170.0</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>180.0</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>190.0</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>200.0</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>210.0</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>220.0</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>230.0</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>240.0</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>250.0</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>260.0</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>270.0</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>280.0</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>290.0</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>300.0</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>310.0</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>320.0</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>330.0</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>340.0</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>350.0</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>360.0</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>370.0</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>380.0</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>390.0</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>400.0</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>410.0</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>420.0</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>430.0</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>440.0</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>450.0</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>460.0</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>470.0</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>480.0</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>490.0</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>500.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet2!$G$3:$G$56</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="54"/>
+                <c:pt idx="0">
+                  <c:v>172.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>168.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>166.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>163.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>161.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>159.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>159.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>163.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>162.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>160.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>159.0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>160.0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>161.0</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>161.0</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>160.0</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>159.0</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>160.0</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>159.0</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>158.0</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>157.0</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>159.0</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>159.0</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>157.0</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>158.0</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>158.0</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>159.0</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>159.0</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>158.0</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>157.0</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>156.0</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>153.0</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>153.0</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>150.0</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>150.0</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>155.0</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>155.0</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>155.0</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>156.0</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>158.0</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>159.0</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>160.0</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>168.0</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>168.0</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>167.0</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>165.0</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>164.0</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>161.0</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>162.0</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>163.0</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>161.0</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>163.0</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>165.0</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>165.0</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>165.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="-2120083176"/>
+        <c:axId val="2111848808"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="-2120083176"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="2111848808"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="2111848808"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="-2120083176"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -707,6 +2850,41 @@
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="3" name="Chart 2"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>342900</xdr:colOff>
+      <xdr:row>58</xdr:row>
+      <xdr:rowOff>25400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>30</xdr:col>
+      <xdr:colOff>749300</xdr:colOff>
+      <xdr:row>114</xdr:row>
+      <xdr:rowOff>88900</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -1048,8 +3226,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AE13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1954,4 +4132,1271 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G56"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A38" workbookViewId="0">
+      <selection activeCell="AH80" sqref="AH80"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetData>
+    <row r="1" spans="1:7">
+      <c r="A1" s="1"/>
+      <c r="B1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+      <c r="E1" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F1" s="2"/>
+      <c r="G1" s="2"/>
+    </row>
+    <row r="2" spans="1:7">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F2" t="s">
+        <v>2</v>
+      </c>
+      <c r="G2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3">
+        <v>154</v>
+      </c>
+      <c r="C3">
+        <v>159</v>
+      </c>
+      <c r="D3">
+        <v>163</v>
+      </c>
+      <c r="E3">
+        <v>139</v>
+      </c>
+      <c r="F3">
+        <v>155</v>
+      </c>
+      <c r="G3">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
+      <c r="A4">
+        <v>10</v>
+      </c>
+      <c r="B4">
+        <v>157</v>
+      </c>
+      <c r="C4">
+        <v>158</v>
+      </c>
+      <c r="D4">
+        <v>160</v>
+      </c>
+      <c r="E4">
+        <v>164</v>
+      </c>
+      <c r="F4">
+        <v>166</v>
+      </c>
+      <c r="G4">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
+      <c r="A5">
+        <v>20</v>
+      </c>
+      <c r="B5">
+        <v>152</v>
+      </c>
+      <c r="C5">
+        <v>152</v>
+      </c>
+      <c r="D5">
+        <v>154</v>
+      </c>
+      <c r="E5">
+        <v>163</v>
+      </c>
+      <c r="F5">
+        <v>164</v>
+      </c>
+      <c r="G5">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
+      <c r="A6">
+        <v>30</v>
+      </c>
+      <c r="B6">
+        <v>152</v>
+      </c>
+      <c r="C6">
+        <v>153</v>
+      </c>
+      <c r="D6">
+        <v>154</v>
+      </c>
+      <c r="E6">
+        <v>156</v>
+      </c>
+      <c r="F6">
+        <v>160</v>
+      </c>
+      <c r="G6">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7">
+      <c r="A7">
+        <v>40</v>
+      </c>
+      <c r="B7">
+        <v>152</v>
+      </c>
+      <c r="C7">
+        <v>153</v>
+      </c>
+      <c r="D7">
+        <v>154</v>
+      </c>
+      <c r="E7">
+        <v>158</v>
+      </c>
+      <c r="F7">
+        <v>160</v>
+      </c>
+      <c r="G7">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7">
+      <c r="A8">
+        <v>50</v>
+      </c>
+      <c r="B8">
+        <v>152</v>
+      </c>
+      <c r="C8">
+        <v>153</v>
+      </c>
+      <c r="D8">
+        <v>155</v>
+      </c>
+      <c r="E8">
+        <v>158</v>
+      </c>
+      <c r="F8">
+        <v>158</v>
+      </c>
+      <c r="G8">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7">
+      <c r="A9">
+        <v>60</v>
+      </c>
+      <c r="B9">
+        <v>152</v>
+      </c>
+      <c r="C9">
+        <v>153</v>
+      </c>
+      <c r="D9">
+        <v>156</v>
+      </c>
+      <c r="E9">
+        <v>158</v>
+      </c>
+      <c r="F9">
+        <v>158</v>
+      </c>
+      <c r="G9">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7">
+      <c r="A10">
+        <v>70</v>
+      </c>
+      <c r="B10">
+        <v>151</v>
+      </c>
+      <c r="C10">
+        <v>152</v>
+      </c>
+      <c r="D10">
+        <v>154</v>
+      </c>
+      <c r="E10">
+        <v>159</v>
+      </c>
+      <c r="F10">
+        <v>159</v>
+      </c>
+      <c r="G10">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7">
+      <c r="A11">
+        <v>80</v>
+      </c>
+      <c r="B11">
+        <v>154</v>
+      </c>
+      <c r="C11">
+        <v>154</v>
+      </c>
+      <c r="D11">
+        <v>155</v>
+      </c>
+      <c r="E11">
+        <v>159</v>
+      </c>
+      <c r="F11">
+        <v>160</v>
+      </c>
+      <c r="G11">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7">
+      <c r="A12">
+        <v>90</v>
+      </c>
+      <c r="B12">
+        <v>154</v>
+      </c>
+      <c r="C12">
+        <v>154</v>
+      </c>
+      <c r="D12">
+        <v>155</v>
+      </c>
+      <c r="E12">
+        <v>158</v>
+      </c>
+      <c r="F12">
+        <v>158</v>
+      </c>
+      <c r="G12">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7">
+      <c r="A13">
+        <v>100</v>
+      </c>
+      <c r="B13">
+        <v>153</v>
+      </c>
+      <c r="C13">
+        <v>154</v>
+      </c>
+      <c r="D13">
+        <v>155</v>
+      </c>
+      <c r="E13">
+        <v>158</v>
+      </c>
+      <c r="F13">
+        <v>158</v>
+      </c>
+      <c r="G13">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7">
+      <c r="A14">
+        <v>110</v>
+      </c>
+      <c r="B14">
+        <v>151</v>
+      </c>
+      <c r="C14">
+        <v>152</v>
+      </c>
+      <c r="D14">
+        <v>154</v>
+      </c>
+      <c r="E14">
+        <v>159</v>
+      </c>
+      <c r="F14">
+        <v>159</v>
+      </c>
+      <c r="G14">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7">
+      <c r="A15">
+        <v>120</v>
+      </c>
+      <c r="B15">
+        <v>150</v>
+      </c>
+      <c r="C15">
+        <v>150</v>
+      </c>
+      <c r="D15">
+        <v>151</v>
+      </c>
+      <c r="E15">
+        <v>159</v>
+      </c>
+      <c r="F15">
+        <v>159</v>
+      </c>
+      <c r="G15">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7">
+      <c r="A16">
+        <v>130</v>
+      </c>
+      <c r="B16">
+        <v>151</v>
+      </c>
+      <c r="C16">
+        <v>151</v>
+      </c>
+      <c r="D16">
+        <v>152</v>
+      </c>
+      <c r="E16">
+        <v>159</v>
+      </c>
+      <c r="F16">
+        <v>160</v>
+      </c>
+      <c r="G16">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7">
+      <c r="A17">
+        <v>140</v>
+      </c>
+      <c r="B17">
+        <v>148</v>
+      </c>
+      <c r="C17">
+        <v>148</v>
+      </c>
+      <c r="D17">
+        <v>150</v>
+      </c>
+      <c r="E17">
+        <v>159</v>
+      </c>
+      <c r="F17">
+        <v>159</v>
+      </c>
+      <c r="G17">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7">
+      <c r="A18">
+        <v>150</v>
+      </c>
+      <c r="B18">
+        <v>147</v>
+      </c>
+      <c r="C18">
+        <v>147</v>
+      </c>
+      <c r="D18">
+        <v>148</v>
+      </c>
+      <c r="E18">
+        <v>158</v>
+      </c>
+      <c r="F18">
+        <v>158</v>
+      </c>
+      <c r="G18">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7">
+      <c r="A19">
+        <v>160</v>
+      </c>
+      <c r="B19">
+        <v>143</v>
+      </c>
+      <c r="C19">
+        <v>145</v>
+      </c>
+      <c r="D19">
+        <v>146</v>
+      </c>
+      <c r="E19">
+        <v>157</v>
+      </c>
+      <c r="F19">
+        <v>158</v>
+      </c>
+      <c r="G19">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7">
+      <c r="A20">
+        <v>170</v>
+      </c>
+      <c r="B20">
+        <v>143</v>
+      </c>
+      <c r="C20">
+        <v>144</v>
+      </c>
+      <c r="D20">
+        <v>145</v>
+      </c>
+      <c r="E20">
+        <v>158</v>
+      </c>
+      <c r="F20">
+        <v>158</v>
+      </c>
+      <c r="G20">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7">
+      <c r="A21">
+        <v>180</v>
+      </c>
+      <c r="B21">
+        <v>145</v>
+      </c>
+      <c r="C21">
+        <v>145</v>
+      </c>
+      <c r="D21">
+        <v>146</v>
+      </c>
+      <c r="E21">
+        <v>157</v>
+      </c>
+      <c r="F21">
+        <v>157</v>
+      </c>
+      <c r="G21">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7">
+      <c r="A22">
+        <v>190</v>
+      </c>
+      <c r="B22">
+        <v>146</v>
+      </c>
+      <c r="C22">
+        <v>146</v>
+      </c>
+      <c r="D22">
+        <v>148</v>
+      </c>
+      <c r="E22">
+        <v>156</v>
+      </c>
+      <c r="F22">
+        <v>156</v>
+      </c>
+      <c r="G22">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7">
+      <c r="A23">
+        <v>200</v>
+      </c>
+      <c r="B23">
+        <v>146</v>
+      </c>
+      <c r="C23">
+        <v>147</v>
+      </c>
+      <c r="D23">
+        <v>149</v>
+      </c>
+      <c r="E23">
+        <v>156</v>
+      </c>
+      <c r="F23">
+        <v>157</v>
+      </c>
+      <c r="G23">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7">
+      <c r="A24">
+        <v>210</v>
+      </c>
+      <c r="B24">
+        <v>147</v>
+      </c>
+      <c r="C24">
+        <v>148</v>
+      </c>
+      <c r="D24">
+        <v>149</v>
+      </c>
+      <c r="E24">
+        <v>154</v>
+      </c>
+      <c r="F24">
+        <v>156</v>
+      </c>
+      <c r="G24">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7">
+      <c r="A25">
+        <v>220</v>
+      </c>
+      <c r="B25">
+        <v>148</v>
+      </c>
+      <c r="C25">
+        <v>148</v>
+      </c>
+      <c r="D25">
+        <v>149</v>
+      </c>
+      <c r="E25">
+        <v>155</v>
+      </c>
+      <c r="F25">
+        <v>156</v>
+      </c>
+      <c r="G25">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7">
+      <c r="A26">
+        <v>230</v>
+      </c>
+      <c r="B26">
+        <v>148</v>
+      </c>
+      <c r="C26">
+        <v>148</v>
+      </c>
+      <c r="D26">
+        <v>150</v>
+      </c>
+      <c r="E26">
+        <v>155</v>
+      </c>
+      <c r="F26">
+        <v>156</v>
+      </c>
+      <c r="G26">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7">
+      <c r="A27">
+        <v>240</v>
+      </c>
+      <c r="B27">
+        <v>147</v>
+      </c>
+      <c r="C27">
+        <v>148</v>
+      </c>
+      <c r="D27">
+        <v>150</v>
+      </c>
+      <c r="E27">
+        <v>157</v>
+      </c>
+      <c r="F27">
+        <v>157</v>
+      </c>
+      <c r="G27">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7">
+      <c r="A28">
+        <v>250</v>
+      </c>
+      <c r="B28">
+        <v>147</v>
+      </c>
+      <c r="C28">
+        <v>147</v>
+      </c>
+      <c r="D28">
+        <v>148</v>
+      </c>
+      <c r="E28">
+        <v>157</v>
+      </c>
+      <c r="F28">
+        <v>158</v>
+      </c>
+      <c r="G28">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7">
+      <c r="A29">
+        <v>260</v>
+      </c>
+      <c r="B29">
+        <v>145</v>
+      </c>
+      <c r="C29">
+        <v>146</v>
+      </c>
+      <c r="D29">
+        <v>147</v>
+      </c>
+      <c r="E29">
+        <v>157</v>
+      </c>
+      <c r="F29">
+        <v>157</v>
+      </c>
+      <c r="G29">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7">
+      <c r="A30">
+        <v>270</v>
+      </c>
+      <c r="B30">
+        <v>142</v>
+      </c>
+      <c r="C30">
+        <v>143</v>
+      </c>
+      <c r="D30">
+        <v>144</v>
+      </c>
+      <c r="E30">
+        <v>156</v>
+      </c>
+      <c r="F30">
+        <v>156</v>
+      </c>
+      <c r="G30">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7">
+      <c r="A31">
+        <v>280</v>
+      </c>
+      <c r="B31">
+        <v>142</v>
+      </c>
+      <c r="C31">
+        <v>142</v>
+      </c>
+      <c r="D31">
+        <v>143</v>
+      </c>
+      <c r="E31">
+        <v>156</v>
+      </c>
+      <c r="F31">
+        <v>156</v>
+      </c>
+      <c r="G31">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7">
+      <c r="A32">
+        <v>290</v>
+      </c>
+      <c r="B32">
+        <v>142</v>
+      </c>
+      <c r="C32">
+        <v>147</v>
+      </c>
+      <c r="D32">
+        <v>150</v>
+      </c>
+      <c r="E32">
+        <v>155</v>
+      </c>
+      <c r="F32">
+        <v>155</v>
+      </c>
+      <c r="G32">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7">
+      <c r="A33">
+        <v>300</v>
+      </c>
+      <c r="B33">
+        <v>145</v>
+      </c>
+      <c r="C33">
+        <v>148</v>
+      </c>
+      <c r="D33">
+        <v>151</v>
+      </c>
+      <c r="E33">
+        <v>149</v>
+      </c>
+      <c r="F33">
+        <v>151</v>
+      </c>
+      <c r="G33">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7">
+      <c r="A34">
+        <v>310</v>
+      </c>
+      <c r="B34">
+        <v>146</v>
+      </c>
+      <c r="C34">
+        <v>147</v>
+      </c>
+      <c r="D34">
+        <v>150</v>
+      </c>
+      <c r="E34">
+        <v>150</v>
+      </c>
+      <c r="F34">
+        <v>151</v>
+      </c>
+      <c r="G34">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7">
+      <c r="A35">
+        <v>320</v>
+      </c>
+      <c r="B35">
+        <v>147</v>
+      </c>
+      <c r="C35">
+        <v>148</v>
+      </c>
+      <c r="D35">
+        <v>150</v>
+      </c>
+      <c r="E35">
+        <v>144</v>
+      </c>
+      <c r="F35">
+        <v>148</v>
+      </c>
+      <c r="G35">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7">
+      <c r="A36">
+        <v>330</v>
+      </c>
+      <c r="B36">
+        <v>147</v>
+      </c>
+      <c r="C36">
+        <v>147</v>
+      </c>
+      <c r="D36">
+        <v>149</v>
+      </c>
+      <c r="E36">
+        <v>143</v>
+      </c>
+      <c r="F36">
+        <v>147</v>
+      </c>
+      <c r="G36">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7">
+      <c r="A37">
+        <v>340</v>
+      </c>
+      <c r="B37">
+        <v>148</v>
+      </c>
+      <c r="C37">
+        <v>149</v>
+      </c>
+      <c r="D37">
+        <v>151</v>
+      </c>
+      <c r="E37">
+        <v>147</v>
+      </c>
+      <c r="F37">
+        <v>149</v>
+      </c>
+      <c r="G37">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7">
+      <c r="A38">
+        <v>350</v>
+      </c>
+      <c r="B38">
+        <v>150</v>
+      </c>
+      <c r="C38">
+        <v>151</v>
+      </c>
+      <c r="D38">
+        <v>153</v>
+      </c>
+      <c r="E38">
+        <v>152</v>
+      </c>
+      <c r="F38">
+        <v>153</v>
+      </c>
+      <c r="G38">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7">
+      <c r="A39">
+        <v>360</v>
+      </c>
+      <c r="B39">
+        <v>150</v>
+      </c>
+      <c r="C39">
+        <v>151</v>
+      </c>
+      <c r="D39">
+        <v>153</v>
+      </c>
+      <c r="E39">
+        <v>152</v>
+      </c>
+      <c r="F39">
+        <v>154</v>
+      </c>
+      <c r="G39">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7">
+      <c r="A40">
+        <v>370</v>
+      </c>
+      <c r="B40">
+        <v>149</v>
+      </c>
+      <c r="C40">
+        <v>150</v>
+      </c>
+      <c r="D40">
+        <v>151</v>
+      </c>
+      <c r="E40">
+        <v>153</v>
+      </c>
+      <c r="F40">
+        <v>155</v>
+      </c>
+      <c r="G40">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7">
+      <c r="A41">
+        <v>380</v>
+      </c>
+      <c r="B41">
+        <v>147</v>
+      </c>
+      <c r="C41">
+        <v>148</v>
+      </c>
+      <c r="D41">
+        <v>150</v>
+      </c>
+      <c r="E41">
+        <v>155</v>
+      </c>
+      <c r="F41">
+        <v>156</v>
+      </c>
+      <c r="G41">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7">
+      <c r="A42">
+        <v>390</v>
+      </c>
+      <c r="B42">
+        <v>147</v>
+      </c>
+      <c r="C42">
+        <v>149</v>
+      </c>
+      <c r="D42">
+        <v>155</v>
+      </c>
+      <c r="E42">
+        <v>156</v>
+      </c>
+      <c r="F42">
+        <v>157</v>
+      </c>
+      <c r="G42">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7">
+      <c r="A43">
+        <v>400</v>
+      </c>
+      <c r="B43">
+        <v>152</v>
+      </c>
+      <c r="C43">
+        <v>153</v>
+      </c>
+      <c r="D43">
+        <v>155</v>
+      </c>
+      <c r="E43">
+        <v>156</v>
+      </c>
+      <c r="F43">
+        <v>158</v>
+      </c>
+      <c r="G43">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7">
+      <c r="A44">
+        <v>410</v>
+      </c>
+      <c r="B44">
+        <v>150</v>
+      </c>
+      <c r="C44">
+        <v>152</v>
+      </c>
+      <c r="D44">
+        <v>153</v>
+      </c>
+      <c r="E44">
+        <v>157</v>
+      </c>
+      <c r="F44">
+        <v>164</v>
+      </c>
+      <c r="G44">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7">
+      <c r="A45">
+        <v>420</v>
+      </c>
+      <c r="B45">
+        <v>146</v>
+      </c>
+      <c r="C45">
+        <v>148</v>
+      </c>
+      <c r="D45">
+        <v>150</v>
+      </c>
+      <c r="E45">
+        <v>166</v>
+      </c>
+      <c r="F45">
+        <v>167</v>
+      </c>
+      <c r="G45">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7">
+      <c r="A46">
+        <v>430</v>
+      </c>
+      <c r="B46">
+        <v>147</v>
+      </c>
+      <c r="C46">
+        <v>148</v>
+      </c>
+      <c r="D46">
+        <v>149</v>
+      </c>
+      <c r="E46">
+        <v>164</v>
+      </c>
+      <c r="F46">
+        <v>166</v>
+      </c>
+      <c r="G46">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7">
+      <c r="A47">
+        <v>440</v>
+      </c>
+      <c r="B47">
+        <v>148</v>
+      </c>
+      <c r="C47">
+        <v>150</v>
+      </c>
+      <c r="D47">
+        <v>153</v>
+      </c>
+      <c r="E47">
+        <v>164</v>
+      </c>
+      <c r="F47">
+        <v>164</v>
+      </c>
+      <c r="G47">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7">
+      <c r="A48">
+        <v>450</v>
+      </c>
+      <c r="B48">
+        <v>152</v>
+      </c>
+      <c r="C48">
+        <v>154</v>
+      </c>
+      <c r="D48">
+        <v>156</v>
+      </c>
+      <c r="E48">
+        <v>160</v>
+      </c>
+      <c r="F48">
+        <v>162</v>
+      </c>
+      <c r="G48">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7">
+      <c r="A49">
+        <v>460</v>
+      </c>
+      <c r="B49">
+        <v>156</v>
+      </c>
+      <c r="C49">
+        <v>157</v>
+      </c>
+      <c r="D49">
+        <v>158</v>
+      </c>
+      <c r="E49">
+        <v>159</v>
+      </c>
+      <c r="F49">
+        <v>160</v>
+      </c>
+      <c r="G49">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7">
+      <c r="A50">
+        <v>470</v>
+      </c>
+      <c r="B50">
+        <v>154</v>
+      </c>
+      <c r="C50">
+        <v>155</v>
+      </c>
+      <c r="D50">
+        <v>156</v>
+      </c>
+      <c r="E50">
+        <v>159</v>
+      </c>
+      <c r="F50">
+        <v>160</v>
+      </c>
+      <c r="G50">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7">
+      <c r="A51">
+        <v>480</v>
+      </c>
+      <c r="B51">
+        <v>154</v>
+      </c>
+      <c r="C51">
+        <v>154</v>
+      </c>
+      <c r="D51">
+        <v>156</v>
+      </c>
+      <c r="E51">
+        <v>160</v>
+      </c>
+      <c r="F51">
+        <v>161</v>
+      </c>
+      <c r="G51">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7">
+      <c r="A52">
+        <v>490</v>
+      </c>
+      <c r="B52">
+        <v>155</v>
+      </c>
+      <c r="C52">
+        <v>155</v>
+      </c>
+      <c r="D52">
+        <v>156</v>
+      </c>
+      <c r="E52">
+        <v>155</v>
+      </c>
+      <c r="F52">
+        <v>158</v>
+      </c>
+      <c r="G52">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7">
+      <c r="A53">
+        <v>500</v>
+      </c>
+      <c r="B53">
+        <v>154</v>
+      </c>
+      <c r="C53">
+        <v>155</v>
+      </c>
+      <c r="D53">
+        <v>157</v>
+      </c>
+      <c r="E53">
+        <v>161</v>
+      </c>
+      <c r="F53">
+        <v>161</v>
+      </c>
+      <c r="G53">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7">
+      <c r="E54">
+        <v>160</v>
+      </c>
+      <c r="F54">
+        <v>162</v>
+      </c>
+      <c r="G54">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7">
+      <c r="E55">
+        <v>161</v>
+      </c>
+      <c r="F55">
+        <v>163</v>
+      </c>
+      <c r="G55">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7">
+      <c r="E56">
+        <v>160</v>
+      </c>
+      <c r="F56">
+        <v>163</v>
+      </c>
+      <c r="G56">
+        <v>165</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="B1:D1"/>
+    <mergeCell ref="E1:G1"/>
+  </mergeCells>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <drawing r:id="rId1"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
 </file>
</xml_diff>